<commit_message>
Corrected duplicate screen assignment
</commit_message>
<xml_diff>
--- a/Borus.xlsx
+++ b/Borus.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/egrstudent/GitHub/atmRepo/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7515"/>
+    <workbookView xWindow="17820" yWindow="8500" windowWidth="14380" windowHeight="7520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -123,136 +126,136 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -558,18 +561,18 @@
   <dimension ref="B1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="79.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="79.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -580,18 +583,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="8">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -600,7 +603,7 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
@@ -609,7 +612,7 @@
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -618,7 +621,7 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -629,7 +632,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
@@ -638,7 +641,7 @@
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
@@ -647,7 +650,7 @@
       </c>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -658,7 +661,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
@@ -667,7 +670,7 @@
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>10</v>
       </c>

</xml_diff>